<commit_message>
lib in cbB complex deperturbation
</commit_message>
<xml_diff>
--- a/lib/korek/state1.xlsx
+++ b/lib/korek/state1.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
   <si>
     <t>R</t>
   </si>
@@ -57,7 +63,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -69,16 +75,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -92,15 +100,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="true"/>
-    <col min="2" max="2" width="9.42578125" customWidth="true"/>
+    <col min="2" max="2" width="9.37890625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">

</xml_diff>